<commit_message>
updated the readme with dataset link and requirements; removed metadata from xlsx files; corrected small bugs inserted during latest commit
</commit_message>
<xml_diff>
--- a/results_tables_paper/auc_classification_etsaliencymap_paper.xlsx
+++ b/results_tables_paper/auc_classification_etsaliencymap_paper.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ric_b\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5983689D-5CD5-46BC-9B13-F953F848F164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{A983E292-5846-43F8-B89B-5515B1BE139F}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="2" r:id="rId1"/>
-    <sheet name="results_all_models" sheetId="1" r:id="rId2"/>
+    <sheet name="summary" sheetId="2" r:id="rId4"/>
+    <sheet name="results_all_models" sheetId="1" r:id="rId5"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,7 +122,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -147,25 +153,119 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -178,7 +278,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ricardo Bigolin Lanfredi" refreshedDate="44407.642625810186" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="10" xr:uid="{4F856ED3-3A27-4F73-8CF8-65C2FB7ABAFF}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" refreshedBy="Ricardo Bigolin Lanfredi" refreshedDate="44407.642625810186" recordCount="10">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:Q11" sheet="results_all_models"/>
   </cacheSource>
@@ -190,59 +290,54 @@
       </sharedItems>
     </cacheField>
     <cacheField name="modeln" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" count="0"/>
     </cacheField>
     <cacheField name="No Finding" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.80507458399999998" maxValue="0.814270194"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Enlarged Cardiomediastinum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.69396181999999995" maxValue="0.72072277200000001"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Cardiomegaly" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.75485553800000005" maxValue="0.76730571299999994"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Lung Lesion" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.63896421400000003" maxValue="0.67960546899999996"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Lung Opacity" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.70120344400000001" maxValue="0.71461334499999996"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Edema" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.82576844000000005" maxValue="0.83261565699999995"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Consolidation" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.74579146299999999" maxValue="0.76392816799999996"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Pneumonia" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.70002432299999995" maxValue="0.72579996599999996"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Atelectasis" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.74293673000000005" maxValue="0.75288272199999995"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Pneumothorax" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.81288099000000003" maxValue="0.85339195700000003"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Pleural Effusion" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.86763527900000004" maxValue="0.87348475699999995"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Pleural Other" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.83369310600000002" maxValue="0.86691767099999995"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Fracture" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.65926299799999999" maxValue="0.73236601400000001"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="Support Devices" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.85368646800000003" maxValue="0.86803002500000004"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
     <cacheField name="auc" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.76511866692857133" maxValue="0.7782435653571429"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
     </cacheField>
   </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
 </pivotCacheDefinition>
 </file>
 
@@ -442,7 +537,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AE6BAE0B-A6DC-49BA-B1BD-4B750E65AD5D}" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="1" preserveFormatting="1" useAutoFormatting="1" itemPrintTitles="1" outline="1" outlineData="1" createdVersion="7" updatedVersion="7" indent="0" multipleFieldFilters="0" showMemberPropertyTips="1">
   <location ref="A1:C4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
@@ -501,7 +596,7 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+      <x14:pivotTableDefinition hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
@@ -806,21 +901,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACACD10B-717F-436D-BC90-B0932B94983A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACACD10B-717F-436D-BC90-B0932B94983A}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.142857142857142" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -832,7 +927,7 @@
       </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -840,11 +935,11 @@
         <v>0.76859601789999998</v>
       </c>
       <c r="C2" s="1">
-        <v>3.9774258314472346E-3</v>
+        <v>0.0039774258314472346</v>
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -852,10 +947,10 @@
         <v>0.77353547061428574</v>
       </c>
       <c r="C3" s="1">
-        <v>2.9357705092364697E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.0029357705092364697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -863,31 +958,32 @@
         <v>0.77106574425714292</v>
       </c>
       <c r="C4" s="1">
-        <v>4.1998695972021256E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.0041998695972021256</v>
+      </c>
+    </row>
+    <row r="5" spans="11:11" ht="15">
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="11:11" ht="15">
       <c r="K6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E1F024-68BF-48CB-A33C-6117400FB6CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E1F024-68BF-48CB-A33C-6117400FB6CE}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -990,11 +1086,11 @@
         <v>0.86678530399999998</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q10" si="0">AVERAGE(C2:P2)</f>
+        <f t="shared" si="0" ref="Q2:Q10">AVERAGE(C2:P2)</f>
         <v>0.77287775250000024</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1144,7 @@
         <v>0.7782435653571429</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1198,7 @@
         <v>0.77418683364285723</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1156,7 +1252,7 @@
         <v>0.77073806242857124</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1306,7 @@
         <v>0.77163113914285719</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1360,7 @@
         <v>0.76669788764285707</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1318,7 +1414,7 @@
         <v>0.76511866692857133</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1372,7 +1468,7 @@
         <v>0.76989873921428575</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1522,7 @@
         <v>0.77496795014285702</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1482,5 +1578,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed the calculations that are not included in the paper; updated tables to include confidence intervals
</commit_message>
<xml_diff>
--- a/results_tables_paper/auc_classification_etsaliencymap_paper.xlsx
+++ b/results_tables_paper/auc_classification_etsaliencymap_paper.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ric_b\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\projects\ambuj\change_github_for_imimic\etsaliencymaps\results_tables_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60FE69D-48A0-42D4-981E-CC85C518C30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="2" r:id="rId4"/>
-    <sheet name="results_all_models" sheetId="1" r:id="rId5"/>
+    <sheet name="summary" sheetId="2" r:id="rId1"/>
+    <sheet name="results_all_models" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId2"/>
+    <pivotCache cacheId="133" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>model</t>
   </si>
@@ -107,13 +107,19 @@
   </si>
   <si>
     <t>StdDev of auc</t>
+  </si>
+  <si>
+    <t>lower interval 95%</t>
+  </si>
+  <si>
+    <t>upper interval 95%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,13 +128,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -153,31 +153,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -186,86 +164,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -278,7 +184,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" refreshedBy="Ricardo Bigolin Lanfredi" refreshedDate="44407.642625810186" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ricardo Bigolin Lanfredi" refreshedDate="44407.642625810186" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="10" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:Q11" sheet="results_all_models"/>
   </cacheSource>
@@ -290,54 +196,59 @@
       </sharedItems>
     </cacheField>
     <cacheField name="modeln" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1"/>
     </cacheField>
     <cacheField name="No Finding" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Enlarged Cardiomediastinum" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Cardiomegaly" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Lung Lesion" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Lung Opacity" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Edema" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Consolidation" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Pneumonia" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Atelectasis" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Pneumothorax" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Pleural Effusion" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Pleural Other" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Fracture" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="Support Devices" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
     <cacheField name="auc" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" count="0"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1"/>
     </cacheField>
   </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
 </pivotCacheDefinition>
 </file>
 
@@ -537,7 +448,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" showMissing="1" preserveFormatting="1" useAutoFormatting="1" itemPrintTitles="1" outline="1" outlineData="1" createdVersion="7" updatedVersion="7" indent="0" multipleFieldFilters="0" showMemberPropertyTips="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable3" cacheId="133" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:C4" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
@@ -596,7 +507,7 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition hideValuesRow="1"/>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
@@ -901,21 +812,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACACD10B-717F-436D-BC90-B0932B94983A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACACD10B-717F-436D-BC90-B0932B94983A}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.142857142857142" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.142857142857142" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.142857142857142" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -925,9 +836,15 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -935,11 +852,19 @@
         <v>0.76859601789999998</v>
       </c>
       <c r="C2" s="1">
-        <v>0.0039774258314472346</v>
+        <v>3.9774258314472346E-3</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2/SQRT(5)*1.96</f>
+        <v>0.76510965044244472</v>
+      </c>
+      <c r="E2">
+        <f>B2+C2/SQRT(5)*1.96</f>
+        <v>0.77208238535755525</v>
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -947,10 +872,18 @@
         <v>0.77353547061428574</v>
       </c>
       <c r="C3" s="1">
-        <v>0.0029357705092364697</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15">
+        <v>2.9357705092364697E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <f>B3-C3/SQRT(5)*1.96</f>
+        <v>0.77096215430368886</v>
+      </c>
+      <c r="E3" s="2">
+        <f>B3+C3/SQRT(5)*1.96</f>
+        <v>0.77610878692488261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -958,13 +891,13 @@
         <v>0.77106574425714292</v>
       </c>
       <c r="C4" s="1">
-        <v>0.0041998695972021256</v>
-      </c>
-    </row>
-    <row r="5" spans="11:11" ht="15">
+        <v>4.1998695972021256E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="11:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K6" s="4"/>
     </row>
   </sheetData>
@@ -974,16 +907,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E1F024-68BF-48CB-A33C-6117400FB6CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E1F024-68BF-48CB-A33C-6117400FB6CE}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="P28" sqref="P28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1086,11 +1019,11 @@
         <v>0.86678530399999998</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="0" ref="Q2:Q10">AVERAGE(C2:P2)</f>
+        <f t="shared" ref="Q2:Q10" si="0">AVERAGE(C2:P2)</f>
         <v>0.77287775250000024</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1144,7 +1077,7 @@
         <v>0.7782435653571429</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1198,7 +1131,7 @@
         <v>0.77418683364285723</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1185,7 @@
         <v>0.77073806242857124</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1306,7 +1239,7 @@
         <v>0.77163113914285719</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1293,7 @@
         <v>0.76669788764285707</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1414,7 +1347,7 @@
         <v>0.76511866692857133</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1401,7 @@
         <v>0.76989873921428575</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1522,7 +1455,7 @@
         <v>0.77496795014285702</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>

</xml_diff>